<commit_message>
Prevent sample submission without project. Block pooling and experiment without project. Template and tests adaptations.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_submission_v4_0_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_submission_v4_0_0.xlsx
@@ -359,7 +359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="2951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3140" uniqueCount="2951">
   <si>
     <t xml:space="preserve">SAMPLE SUBMISSION</t>
   </si>
@@ -9881,9 +9881,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1558440</xdr:colOff>
+      <xdr:colOff>1557720</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>46080</xdr:rowOff>
+      <xdr:rowOff>45360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -9898,7 +9898,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="76320" y="28440"/>
-          <a:ext cx="1482120" cy="541440"/>
+          <a:ext cx="1481400" cy="540720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9964,7 +9964,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="27.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="17.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="16.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10008,10 +10008,16 @@
         <v>5</v>
       </c>
       <c r="I6" s="7"/>
+      <c r="J6" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="T6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="V6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="W6" s="6" t="s">
         <v>4</v>
       </c>
       <c r="AA6" s="8"/>

</xml_diff>